<commit_message>
Update Keyword Low Competition
</commit_message>
<xml_diff>
--- a/LOW COMPETITION Keyword Contoh.xlsx
+++ b/LOW COMPETITION Keyword Contoh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\INTERNET MARKETING\Keyword\contoh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\INTERNET MARKETING\AGC\Keyword\contoh\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -482,14 +482,15 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -513,519 +514,535 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
+      <c r="A2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="1">
-        <f t="shared" ref="B2:B5" si="0">LEN(A2)-LEN(SUBSTITUTE(A2," ",""))+1</f>
-        <v>7</v>
-      </c>
-      <c r="C2" s="1">
+        <f>LEN(TRIM(A2))-LEN(SUBSTITUTE(A2," ",""))+1</f>
+        <v>9</v>
+      </c>
+      <c r="C2" s="5">
         <v>170</v>
       </c>
       <c r="D2" s="5">
         <f>E2/30</f>
-        <v>10.666666666666666</v>
-      </c>
-      <c r="E2" s="1">
-        <v>320</v>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="E2" s="5">
+        <v>260</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>LEN(A3)-LEN(SUBSTITUTE(A3," ",""))+1</f>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>480</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D14" si="1">E3/30</f>
-        <v>29.333333333333332</v>
+        <f>E3/30</f>
+        <v>3.6666666666666665</v>
       </c>
       <c r="E3" s="1">
-        <v>880</v>
+        <v>110</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(A4))-LEN(SUBSTITUTE(A4," ",""))+1</f>
         <v>8</v>
       </c>
-      <c r="C4" s="1">
-        <v>480</v>
+      <c r="C4" s="5">
+        <v>140</v>
       </c>
       <c r="D4" s="5">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="E4" s="1">
-        <v>480</v>
+        <f>C4/30</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="E4" s="5">
+        <v>70</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <f>LEN(A5)-LEN(SUBSTITUTE(A5," ",""))+1</f>
         <v>8</v>
       </c>
-      <c r="B5" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
       <c r="C5" s="1">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" si="1"/>
-        <v>8.6666666666666661</v>
+        <f>E5/30</f>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>260</v>
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B15" si="2">LEN(TRIM(A6))-LEN(SUBSTITUTE(A6," ",""))+1</f>
-        <v>9</v>
-      </c>
-      <c r="C6" s="5">
-        <v>170</v>
+        <f>LEN(A6)-LEN(SUBSTITUTE(A6," ",""))+1</f>
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>320</v>
       </c>
       <c r="D6" s="5">
-        <f t="shared" si="1"/>
-        <v>8.6666666666666661</v>
-      </c>
-      <c r="E6" s="5">
-        <v>260</v>
+        <f>E6/30</f>
+        <v>16</v>
+      </c>
+      <c r="E6" s="1">
+        <v>480</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="C7" s="5">
+        <f>LEN(A7)-LEN(SUBSTITUTE(A7," ",""))+1</f>
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>70</v>
+      </c>
+      <c r="D7" s="5">
+        <f>E7/30</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="E7" s="1">
         <v>140</v>
       </c>
-      <c r="D7" s="5">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E7" s="5">
-        <v>210</v>
+      <c r="F7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
+      <c r="A8" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="C8" s="5">
-        <v>260</v>
+        <f>LEN(A8)-LEN(SUBSTITUTE(A8," ",""))+1</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>70</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" si="1"/>
-        <v>8.6666666666666661</v>
-      </c>
-      <c r="E8" s="5">
-        <v>260</v>
+        <f>E8/30</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="E8" s="1">
+        <v>70</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="2"/>
+        <f>LEN(A9)-LEN(SUBSTITUTE(A9," ",""))+1</f>
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>170</v>
+      </c>
+      <c r="D9" s="5">
+        <f>E9/30</f>
         <v>7</v>
       </c>
-      <c r="C9" s="5">
+      <c r="E9" s="1">
         <v>210</v>
       </c>
-      <c r="D9" s="5">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E9" s="5">
-        <v>210</v>
+      <c r="F9">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
+      <c r="A10" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="C10" s="5">
-        <v>260</v>
+        <f>LEN(A10)-LEN(SUBSTITUTE(A10," ",""))+1</f>
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>50</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" si="1"/>
-        <v>19.666666666666668</v>
-      </c>
-      <c r="E10" s="5">
-        <v>590</v>
+        <f>E10/30</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="E10" s="1">
+        <v>140</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="C11" s="5">
-        <v>3600</v>
+        <f>LEN(A11)-LEN(SUBSTITUTE(A11," ",""))+1</f>
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>90</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="1"/>
-        <v>270</v>
-      </c>
-      <c r="E11" s="5">
-        <v>8100</v>
+        <f>E11/30</f>
+        <v>13</v>
+      </c>
+      <c r="E11" s="1">
+        <v>390</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f>LEN(TRIM(A12))-LEN(SUBSTITUTE(A12," ",""))+1</f>
+        <v>9</v>
       </c>
       <c r="C12" s="5">
-        <v>880</v>
+        <v>140</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="1"/>
-        <v>53.333333333333336</v>
+        <f>E12/30</f>
+        <v>7</v>
       </c>
       <c r="E12" s="5">
-        <v>1600</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="C13" s="5">
-        <v>590</v>
+        <f>LEN(A13)-LEN(SUBSTITUTE(A13," ",""))+1</f>
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>480</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="1"/>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="E13" s="5">
-        <v>1000</v>
+        <f>E13/30</f>
+        <v>29.333333333333332</v>
+      </c>
+      <c r="E13" s="1">
+        <v>880</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="C14" s="5">
-        <v>170</v>
+        <f>LEN(A14)-LEN(SUBSTITUTE(A14," ",""))+1</f>
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>480</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" si="1"/>
-        <v>5.666666666666667</v>
-      </c>
-      <c r="E14" s="5">
-        <v>170</v>
+        <f>E14/30</f>
+        <v>16</v>
+      </c>
+      <c r="E14" s="1">
+        <v>480</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="2"/>
+        <f>LEN(A15)-LEN(SUBSTITUTE(A15," ",""))+1</f>
         <v>8</v>
       </c>
-      <c r="C15" s="5">
-        <v>140</v>
+      <c r="C15" s="1">
+        <v>170</v>
       </c>
       <c r="D15" s="5">
-        <f>C15/30</f>
-        <v>4.666666666666667</v>
-      </c>
-      <c r="E15" s="5">
-        <v>70</v>
+        <f>E15/30</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="E15" s="1">
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" ref="B16:B17" si="3">LEN(A16)-LEN(SUBSTITUTE(A16," ",""))+1</f>
-        <v>9</v>
-      </c>
-      <c r="C16" s="1">
-        <v>10</v>
+        <f>LEN(TRIM(A16))-LEN(SUBSTITUTE(A16," ",""))+1</f>
+        <v>8</v>
+      </c>
+      <c r="C16" s="5">
+        <v>260</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" ref="D16:D17" si="4">E16/30</f>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="E16" s="1">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
+        <f>E16/30</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="E16" s="5">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="3"/>
+        <f>LEN(A17)-LEN(SUBSTITUTE(A17," ",""))+1</f>
         <v>8</v>
       </c>
       <c r="C17" s="1">
-        <v>50</v>
+        <v>210</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>E17/30</f>
+        <v>7</v>
       </c>
       <c r="E17" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>21</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" ref="B18:B27" si="5">LEN(A18)-LEN(SUBSTITUTE(A18," ",""))+1</f>
-        <v>8</v>
+        <f>LEN(A18)-LEN(SUBSTITUTE(A18," ",""))+1</f>
+        <v>7</v>
       </c>
       <c r="C18" s="1">
+        <v>170</v>
+      </c>
+      <c r="D18" s="5">
+        <f>E18/30</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="E18" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1">
+        <f>LEN(TRIM(A19))-LEN(SUBSTITUTE(A19," ",""))+1</f>
+        <v>7</v>
+      </c>
+      <c r="C19" s="5">
         <v>210</v>
       </c>
-      <c r="D18" s="5">
-        <f t="shared" ref="D18:D27" si="6">E18/30</f>
+      <c r="D19" s="5">
+        <f>E19/30</f>
         <v>7</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E19" s="5">
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <f>LEN(TRIM(A20))-LEN(SUBSTITUTE(A20," ",""))+1</f>
+        <v>7</v>
+      </c>
+      <c r="C20" s="5">
+        <v>260</v>
+      </c>
+      <c r="D20" s="5">
+        <f>E20/30</f>
+        <v>19.666666666666668</v>
+      </c>
+      <c r="E20" s="5">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1">
+        <f>LEN(TRIM(A21))-LEN(SUBSTITUTE(A21," ",""))+1</f>
+        <v>7</v>
+      </c>
+      <c r="C21" s="5">
+        <v>170</v>
+      </c>
+      <c r="D21" s="5">
+        <f>E21/30</f>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="E21" s="5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <f>LEN(TRIM(A22))-LEN(SUBSTITUTE(A22," ",""))+1</f>
+        <v>6</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3600</v>
+      </c>
+      <c r="D22" s="5">
+        <f>E22/30</f>
+        <v>270</v>
+      </c>
+      <c r="E22" s="5">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1">
-        <f t="shared" si="5"/>
+      <c r="B23" s="1">
+        <f>LEN(A23)-LEN(SUBSTITUTE(A23," ",""))+1</f>
         <v>6</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C23" s="1">
         <v>90</v>
       </c>
-      <c r="D19" s="5">
-        <f t="shared" si="6"/>
+      <c r="D23" s="5">
+        <f>E23/30</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E23" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="1">
-        <f t="shared" si="5"/>
+      <c r="B24" s="1">
+        <f>LEN(A24)-LEN(SUBSTITUTE(A24," ",""))+1</f>
         <v>6</v>
-      </c>
-      <c r="C20" s="1">
-        <v>50</v>
-      </c>
-      <c r="D20" s="5">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="E20" s="1">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="C21" s="1">
-        <v>70</v>
-      </c>
-      <c r="D21" s="5">
-        <f t="shared" si="6"/>
-        <v>24</v>
-      </c>
-      <c r="E21" s="1">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="1">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="C22" s="1">
-        <v>90</v>
-      </c>
-      <c r="D22" s="5">
-        <f t="shared" si="6"/>
-        <v>13</v>
-      </c>
-      <c r="E22" s="1">
-        <v>390</v>
-      </c>
-      <c r="F22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="1">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="C23" s="1">
-        <v>170</v>
-      </c>
-      <c r="D23" s="5">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="E23" s="1">
-        <v>210</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="1">
-        <f t="shared" si="5"/>
-        <v>5</v>
       </c>
       <c r="C24" s="1">
         <v>50</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" si="6"/>
-        <v>4.666666666666667</v>
+        <f>E24/30</f>
+        <v>7</v>
       </c>
       <c r="E24" s="1">
-        <v>140</v>
-      </c>
-      <c r="F24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f>LEN(A25)-LEN(SUBSTITUTE(A25," ",""))+1</f>
+        <v>6</v>
       </c>
       <c r="C25" s="1">
-        <v>320</v>
+        <v>70</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" si="6"/>
+        <f>E25/30</f>
+        <v>24</v>
+      </c>
+      <c r="E25" s="1">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1">
+        <f>LEN(TRIM(A26))-LEN(SUBSTITUTE(A26," ",""))+1</f>
+        <v>5</v>
+      </c>
+      <c r="C26" s="5">
+        <v>880</v>
+      </c>
+      <c r="D26" s="5">
+        <f>E26/30</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="1">
-        <v>480</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="1">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="C26" s="1">
-        <v>70</v>
-      </c>
-      <c r="D26" s="5">
-        <f t="shared" si="6"/>
-        <v>4.666666666666667</v>
-      </c>
-      <c r="E26" s="1">
-        <v>140</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="B27" s="1">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="C27" s="1">
-        <v>70</v>
+        <f>LEN(TRIM(A27))-LEN(SUBSTITUTE(A27," ",""))+1</f>
+        <v>5</v>
+      </c>
+      <c r="C27" s="5">
+        <v>590</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="6"/>
-        <v>2.3333333333333335</v>
-      </c>
-      <c r="E27" s="1">
-        <v>70</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
+        <f>E27/30</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F27"/>
+  <autoFilter ref="A1:F27">
+    <sortState ref="A2:F27">
+      <sortCondition ref="F1:F27"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tambah artikel draft contoh surat lamaran kerja ke sekolah sebagai tata usaha
</commit_message>
<xml_diff>
--- a/LOW COMPETITION Keyword Contoh.xlsx
+++ b/LOW COMPETITION Keyword Contoh.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Keywords</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>DONE ?</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -479,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +499,7 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,8 +518,11 @@
       <c r="F1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -534,8 +543,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -557,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -579,19 +591,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1">
-        <f>LEN(A5)-LEN(SUBSTITUTE(A5," ",""))+1</f>
+        <f t="shared" ref="B5:B11" si="0">LEN(A5)-LEN(SUBSTITUTE(A5," ",""))+1</f>
         <v>8</v>
       </c>
       <c r="C5" s="1">
         <v>50</v>
       </c>
       <c r="D5" s="5">
-        <f>E5/30</f>
+        <f t="shared" ref="D5:D27" si="1">E5/30</f>
         <v>1</v>
       </c>
       <c r="E5" s="1">
@@ -601,19 +613,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1">
-        <f>LEN(A6)-LEN(SUBSTITUTE(A6," ",""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>320</v>
       </c>
       <c r="D6" s="5">
-        <f>E6/30</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="E6" s="1">
@@ -623,19 +635,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="1">
-        <f>LEN(A7)-LEN(SUBSTITUTE(A7," ",""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>70</v>
       </c>
       <c r="D7" s="5">
-        <f>E7/30</f>
+        <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
       <c r="E7" s="1">
@@ -645,19 +657,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1">
-        <f>LEN(A8)-LEN(SUBSTITUTE(A8," ",""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C8" s="1">
         <v>70</v>
       </c>
       <c r="D8" s="5">
-        <f>E8/30</f>
+        <f t="shared" si="1"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="E8" s="1">
@@ -667,19 +679,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="1">
-        <f>LEN(A9)-LEN(SUBSTITUTE(A9," ",""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>170</v>
       </c>
       <c r="D9" s="5">
-        <f>E9/30</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E9" s="1">
@@ -689,19 +701,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="1">
-        <f>LEN(A10)-LEN(SUBSTITUTE(A10," ",""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>50</v>
       </c>
       <c r="D10" s="5">
-        <f>E10/30</f>
+        <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
       <c r="E10" s="1">
@@ -711,19 +723,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="1">
-        <f>LEN(A11)-LEN(SUBSTITUTE(A11," ",""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>90</v>
       </c>
       <c r="D11" s="5">
-        <f>E11/30</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E11" s="1">
@@ -733,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -745,14 +757,14 @@
         <v>140</v>
       </c>
       <c r="D12" s="5">
-        <f>E12/30</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E12" s="5">
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -764,14 +776,14 @@
         <v>480</v>
       </c>
       <c r="D13" s="5">
-        <f>E13/30</f>
+        <f t="shared" si="1"/>
         <v>29.333333333333332</v>
       </c>
       <c r="E13" s="1">
         <v>880</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -783,14 +795,14 @@
         <v>480</v>
       </c>
       <c r="D14" s="5">
-        <f>E14/30</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="E14" s="1">
         <v>480</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -802,14 +814,14 @@
         <v>170</v>
       </c>
       <c r="D15" s="5">
-        <f>E15/30</f>
+        <f t="shared" si="1"/>
         <v>8.6666666666666661</v>
       </c>
       <c r="E15" s="1">
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -821,7 +833,7 @@
         <v>260</v>
       </c>
       <c r="D16" s="5">
-        <f>E16/30</f>
+        <f t="shared" si="1"/>
         <v>8.6666666666666661</v>
       </c>
       <c r="E16" s="5">
@@ -840,7 +852,7 @@
         <v>210</v>
       </c>
       <c r="D17" s="5">
-        <f>E17/30</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E17" s="1">
@@ -859,7 +871,7 @@
         <v>170</v>
       </c>
       <c r="D18" s="5">
-        <f>E18/30</f>
+        <f t="shared" si="1"/>
         <v>10.666666666666666</v>
       </c>
       <c r="E18" s="1">
@@ -878,7 +890,7 @@
         <v>210</v>
       </c>
       <c r="D19" s="5">
-        <f>E19/30</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E19" s="5">
@@ -897,7 +909,7 @@
         <v>260</v>
       </c>
       <c r="D20" s="5">
-        <f>E20/30</f>
+        <f t="shared" si="1"/>
         <v>19.666666666666668</v>
       </c>
       <c r="E20" s="5">
@@ -916,7 +928,7 @@
         <v>170</v>
       </c>
       <c r="D21" s="5">
-        <f>E21/30</f>
+        <f t="shared" si="1"/>
         <v>5.666666666666667</v>
       </c>
       <c r="E21" s="5">
@@ -935,7 +947,7 @@
         <v>3600</v>
       </c>
       <c r="D22" s="5">
-        <f>E22/30</f>
+        <f t="shared" si="1"/>
         <v>270</v>
       </c>
       <c r="E22" s="5">
@@ -954,7 +966,7 @@
         <v>90</v>
       </c>
       <c r="D23" s="5">
-        <f>E23/30</f>
+        <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
       <c r="E23" s="1">
@@ -973,7 +985,7 @@
         <v>50</v>
       </c>
       <c r="D24" s="5">
-        <f>E24/30</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E24" s="1">
@@ -992,7 +1004,7 @@
         <v>70</v>
       </c>
       <c r="D25" s="5">
-        <f>E25/30</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="E25" s="1">
@@ -1011,7 +1023,7 @@
         <v>880</v>
       </c>
       <c r="D26" s="5">
-        <f>E26/30</f>
+        <f t="shared" si="1"/>
         <v>53.333333333333336</v>
       </c>
       <c r="E26" s="5">
@@ -1030,7 +1042,7 @@
         <v>590</v>
       </c>
       <c r="D27" s="5">
-        <f>E27/30</f>
+        <f t="shared" si="1"/>
         <v>33.333333333333336</v>
       </c>
       <c r="E27" s="5">

</xml_diff>

<commit_message>
Penambahan draft artikel dan modifikasi source file keyword
</commit_message>
<xml_diff>
--- a/LOW COMPETITION Keyword Contoh.xlsx
+++ b/LOW COMPETITION Keyword Contoh.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Keywords</t>
   </si>
@@ -128,7 +128,13 @@
     <t>DONE ?</t>
   </si>
   <si>
-    <t>y</t>
+    <t>contoh daftar riwayat hidup untuk melamar kerja tulisan tangan</t>
+  </si>
+  <si>
+    <t>contoh daftar riwayat hidup lamaran kerja guru honorer</t>
+  </si>
+  <si>
+    <t>contoh daftar riwayat hidup lulusan smk</t>
   </si>
 </sst>
 </file>
@@ -485,15 +491,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
@@ -543,8 +549,8 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>33</v>
+      <c r="G2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -566,7 +572,7 @@
         <v>110</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -603,13 +609,16 @@
         <v>50</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" ref="D5:D27" si="1">E5/30</f>
+        <f t="shared" ref="D5:D28" si="1">E5/30</f>
         <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>30</v>
       </c>
       <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
     </row>
@@ -654,7 +663,7 @@
         <v>140</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -839,8 +848,14 @@
       <c r="E16" s="5">
         <v>260</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -859,7 +874,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -878,7 +893,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -897,7 +912,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -916,7 +931,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -935,7 +950,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -954,7 +969,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
@@ -972,8 +987,11 @@
       <c r="E23" s="1">
         <v>140</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -991,8 +1009,11 @@
       <c r="E24" s="1">
         <v>210</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1010,8 +1031,11 @@
       <c r="E25" s="1">
         <v>720</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
@@ -1030,7 +1054,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
@@ -1047,6 +1071,66 @@
       </c>
       <c r="E27" s="5">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" ref="B28" si="2">LEN(TRIM(A28))-LEN(SUBSTITUTE(A28," ",""))+1</f>
+        <v>9</v>
+      </c>
+      <c r="C28" s="1">
+        <v>720</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="1"/>
+        <v>19.666666666666668</v>
+      </c>
+      <c r="E28" s="1">
+        <v>590</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="1">
+        <f>LEN(A29)-LEN(SUBSTITUTE(A29," ",""))+1</f>
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
+        <v>90</v>
+      </c>
+      <c r="D29" s="5">
+        <f>E29/30</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="E29" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="1">
+        <f>LEN(A30)-LEN(SUBSTITUTE(A30," ",""))+1</f>
+        <v>6</v>
+      </c>
+      <c r="C30" s="1">
+        <v>90</v>
+      </c>
+      <c r="D30" s="5">
+        <f>E30/30</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="E30" s="1">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update dan tambah draft article
</commit_message>
<xml_diff>
--- a/LOW COMPETITION Keyword Contoh.xlsx
+++ b/LOW COMPETITION Keyword Contoh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\INTERNET MARKETING\AGC\Keyword\contoh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\INTERNET MARKETING\KEYWORDS\key-contoh\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Keywords</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>contoh daftar riwayat hidup lulusan smk</t>
+  </si>
+  <si>
+    <t>contoh surat lamaran kerja bidan di rumah sakit swasta</t>
+  </si>
+  <si>
+    <t>contoh surat lamaran kerja bidan di klinik bersalin</t>
+  </si>
+  <si>
+    <t>contoh surat lamaran kerja di bidang kesehatan dalam bahasa inggris</t>
+  </si>
+  <si>
+    <t>contoh surat lamaran kerja bidan untuk dinas kesehatan</t>
   </si>
 </sst>
 </file>
@@ -491,15 +503,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
@@ -1131,6 +1143,51 @@
       </c>
       <c r="E30" s="1">
         <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" ref="B31:B34" si="3">LEN(A31)-LEN(SUBSTITUTE(A31," ",""))+1</f>
+        <v>9</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update dan tambah file domain hosting backlink detail
</commit_message>
<xml_diff>
--- a/LOW COMPETITION Keyword Contoh.xlsx
+++ b/LOW COMPETITION Keyword Contoh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\INTERNET MARKETING\AGC\Keyword\contoh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\INTERNET MARKETING\Keyword\contoh\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -493,16 +493,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>